<commit_message>
Update schedule for HT2023
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malla74/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB55893-1B9F-304D-AC56-39E932FA2C53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B5427B-D00B-FB44-B6FE-1883ED251B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20460" yWindow="11220" windowWidth="28880" windowHeight="18860" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
+    <workbookView xWindow="880" yWindow="840" windowWidth="28880" windowHeight="18860" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
   <si>
     <t>date</t>
   </si>
@@ -131,9 +131,6 @@
     <t>Quality control</t>
   </si>
   <si>
-    <t>Markus Mayrhofer</t>
-  </si>
-  <si>
     <t>https://youtu.be/gytTBNSWpFc</t>
   </si>
   <si>
@@ -146,18 +143,12 @@
     <t>NGS tech &amp; challenges</t>
   </si>
   <si>
-    <t>Olga Vinnere Petterson</t>
-  </si>
-  <si>
     <t>https://youtu.be/5sUzkrucL1E</t>
   </si>
   <si>
     <t>NGS Pipelines</t>
   </si>
   <si>
-    <t>Franziska Bonath / Maxime Garcia</t>
-  </si>
-  <si>
     <t>https://youtu.be/6RBhfMvDkSI</t>
   </si>
   <si>
@@ -179,18 +170,12 @@
     <t>RNA-Seq workflow</t>
   </si>
   <si>
-    <t>Dag Ahren / Roy Francis</t>
-  </si>
-  <si>
     <t>https://youtu.be/gC_nslHgSa8</t>
   </si>
   <si>
     <t>Data management practices</t>
   </si>
   <si>
-    <t>Elin Kronander / Stephan Nylinder</t>
-  </si>
-  <si>
     <t>https://youtu.be/PfcrDlhY1zE</t>
   </si>
   <si>
@@ -203,9 +188,6 @@
     <t>Martin Dahlö</t>
   </si>
   <si>
-    <t>Dag Ahrén / Björn Nystedt</t>
-  </si>
-  <si>
     <t>topics/linux/slide_linux_intro.pdf</t>
   </si>
   <si>
@@ -278,29 +260,50 @@
     <t>17/11/2023</t>
   </si>
   <si>
-    <t>KL</t>
-  </si>
-  <si>
-    <t>MR</t>
-  </si>
-  <si>
-    <t>JH,ML</t>
-  </si>
-  <si>
-    <t>AJ,ML</t>
-  </si>
-  <si>
-    <t>VH</t>
-  </si>
-  <si>
     <t>ML,VH</t>
+  </si>
+  <si>
+    <t>Adam Ameur &amp; Johanna Lagensjö</t>
+  </si>
+  <si>
+    <t>Adam Ameur</t>
+  </si>
+  <si>
+    <t>Malin Larsson</t>
+  </si>
+  <si>
+    <t>Roy Francis</t>
+  </si>
+  <si>
+    <t>Elin Kronander</t>
+  </si>
+  <si>
+    <t>GD, LS</t>
+  </si>
+  <si>
+    <t>MR, MP</t>
+  </si>
+  <si>
+    <t>GD, MP</t>
+  </si>
+  <si>
+    <t>KL, MP</t>
+  </si>
+  <si>
+    <t>JH,MM</t>
+  </si>
+  <si>
+    <t>AJ,MM</t>
+  </si>
+  <si>
+    <t>VH, MD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -312,6 +315,20 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -338,10 +355,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -664,7 +684,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+      <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,7 +693,7 @@
     <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="30" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="31.5" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="29.5" bestFit="1" customWidth="1"/>
@@ -699,7 +719,7 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="H1" t="s">
@@ -717,7 +737,7 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
@@ -732,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -746,10 +766,10 @@
         <v>13</v>
       </c>
       <c r="F3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H3" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>14</v>
@@ -766,13 +786,13 @@
         <v>13</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>72</v>
       </c>
       <c r="I4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -797,10 +817,10 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H6" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>17</v>
@@ -817,15 +837,18 @@
         <v>16</v>
       </c>
       <c r="F7" t="s">
-        <v>46</v>
+        <v>41</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="C8" s="1">
         <v>0.375</v>
@@ -837,10 +860,10 @@
         <v>18</v>
       </c>
       <c r="F8" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="H8" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>19</v>
@@ -857,13 +880,13 @@
         <v>18</v>
       </c>
       <c r="F9" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" t="s">
+        <v>41</v>
+      </c>
+      <c r="G9" s="5" t="s">
         <v>73</v>
       </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -877,10 +900,10 @@
         <v>20</v>
       </c>
       <c r="F10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" t="s">
         <v>46</v>
-      </c>
-      <c r="H10" t="s">
-        <v>52</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>21</v>
@@ -908,16 +931,19 @@
         <v>22</v>
       </c>
       <c r="F12" t="s">
+        <v>69</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H12" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" t="s">
+        <v>48</v>
+      </c>
+      <c r="J12" s="2" t="s">
         <v>23</v>
-      </c>
-      <c r="H12" t="s">
-        <v>53</v>
-      </c>
-      <c r="I12" t="s">
-        <v>54</v>
-      </c>
-      <c r="J12" s="2" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -928,16 +954,16 @@
         <v>0.625</v>
       </c>
       <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="F13" t="s">
+        <v>41</v>
+      </c>
+      <c r="H13" t="s">
+        <v>49</v>
+      </c>
+      <c r="J13" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F13" t="s">
-        <v>46</v>
-      </c>
-      <c r="H13" t="s">
-        <v>55</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -948,21 +974,21 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" t="s">
-        <v>72</v>
+        <v>41</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="I14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C15" s="1">
         <v>0.375</v>
@@ -971,19 +997,19 @@
         <v>0.42708333333333331</v>
       </c>
       <c r="E15" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H15" t="s">
+        <v>51</v>
+      </c>
+      <c r="J15" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F15" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" t="s">
-        <v>57</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    </row>
+    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="C16" s="1">
         <v>0.42708333333333331</v>
       </c>
@@ -991,13 +1017,13 @@
         <v>0.45833333333333331</v>
       </c>
       <c r="E16" t="s">
-        <v>27</v>
-      </c>
-      <c r="F16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
         <v>0.45833333333333331</v>
       </c>
@@ -1005,16 +1031,16 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F17" t="s">
-        <v>31</v>
+        <v>28</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>68</v>
       </c>
       <c r="H17" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1036,16 +1062,16 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E19" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F19" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="H19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1056,16 +1082,16 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E20" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G20" t="s">
-        <v>74</v>
+        <v>69</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>76</v>
       </c>
       <c r="I20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1076,12 +1102,12 @@
         <v>0.875</v>
       </c>
       <c r="E21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C22" s="1">
         <v>0.375</v>
@@ -1090,13 +1116,13 @@
         <v>0.39583333333333331</v>
       </c>
       <c r="E22" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>23</v>
+        <v>69</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1107,13 +1133,13 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="E23" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" t="s">
-        <v>75</v>
+        <v>69</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1135,16 +1161,16 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E25" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F25" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="H25" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1155,21 +1181,21 @@
         <v>0.70833333333333337</v>
       </c>
       <c r="E26" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>39</v>
-      </c>
-      <c r="G26" t="s">
-        <v>77</v>
+        <v>70</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>66</v>
       </c>
       <c r="I26" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C27" s="1">
         <v>0.375</v>
@@ -1178,13 +1204,13 @@
         <v>0.48958333333333331</v>
       </c>
       <c r="E27" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F27" t="s">
-        <v>39</v>
-      </c>
-      <c r="G27" t="s">
-        <v>76</v>
+        <v>70</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1206,16 +1232,16 @@
         <v>0.58333333333333337</v>
       </c>
       <c r="E29" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="F29" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="H29" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.2">
@@ -1226,16 +1252,13 @@
         <v>0.59375</v>
       </c>
       <c r="E30" t="s">
-        <v>44</v>
-      </c>
-      <c r="F30" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="H30" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add teacher to NBIS talk
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malla74/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2B5427B-D00B-FB44-B6FE-1883ED251B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD75F970-C367-8544-87C0-F91451F80C2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="880" yWindow="840" windowWidth="28880" windowHeight="18860" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
+    <workbookView xWindow="1820" yWindow="500" windowWidth="28880" windowHeight="18860" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="79">
   <si>
     <t>date</t>
   </si>
@@ -1254,6 +1254,9 @@
       <c r="E30" t="s">
         <v>39</v>
       </c>
+      <c r="F30" t="s">
+        <v>71</v>
+      </c>
       <c r="H30" t="s">
         <v>58</v>
       </c>

</xml_diff>

<commit_message>
Updated introduction slides, Added to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBECB6A8-261E-544E-87AE-CA2C77AE1ADA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{812C6ADD-D396-F84B-A508-1E1E8575759E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1820" yWindow="500" windowWidth="28880" windowHeight="18860" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
+    <workbookView xWindow="1820" yWindow="880" windowWidth="28880" windowHeight="18860" xr2:uid="{4D37F018-551B-CF4D-85BF-2DD74B664EBF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="81">
   <si>
     <t>date</t>
   </si>
@@ -300,6 +300,9 @@
   </si>
   <si>
     <t>GD</t>
+  </si>
+  <si>
+    <t>topics/other/slide_introduction.pdf</t>
   </si>
 </sst>
 </file>
@@ -686,7 +689,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -755,6 +758,9 @@
       </c>
       <c r="F2" t="s">
         <v>41</v>
+      </c>
+      <c r="H2" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Remove zoom link (added in previous commit) from schedule.
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malla74/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C82AFE4E-8197-724C-83F5-50AFF0FB004F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2678187A-7A63-DC42-A63A-0F3D882F9636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14560" yWindow="2720" windowWidth="32280" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14540" yWindow="2700" windowWidth="32280" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -261,14 +261,14 @@
     <t>Elin Kronander / Stephan Nylinder</t>
   </si>
   <si>
-    <t>https://uu-se.zoom.us/j/61968741381?pwd=TUxTaysrWFc2RTloeWh4YkRQNUdNZz09</t>
+    <t>Zoom</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -287,6 +287,13 @@
     <font>
       <sz val="13"/>
       <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -318,7 +325,7 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -705,7 +712,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1296,7 +1303,6 @@
     <hyperlink ref="J25" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
     <hyperlink ref="J29" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
     <hyperlink ref="J30" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
-    <hyperlink ref="B2" r:id="rId14" xr:uid="{4163DCFD-D7CA-564F-A953-69000DBE03E9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Update time for lunch
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malla74/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2678187A-7A63-DC42-A63A-0F3D882F9636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7F2CD8-0481-6E43-8DFB-C72E9769BB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14540" yWindow="2700" windowWidth="32280" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -712,7 +712,7 @@
   <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,7 +828,7 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" s="1">
-        <v>0.48958333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="D5" s="1">
         <v>0.54166666666666696</v>
@@ -942,7 +942,7 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C11" s="1">
-        <v>0.48958333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="D11" s="1">
         <v>0.54166666666666696</v>

</xml_diff>

<commit_message>
Merged ngs sequencing and pipelines sessions
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/malla74/workshop-ngsintro/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7F2CD8-0481-6E43-8DFB-C72E9769BB32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C2C3877-BFFA-5644-B5E1-ADCB5DD5AEC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14540" yWindow="2700" windowWidth="32280" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28760" yWindow="2100" windowWidth="32280" windowHeight="21580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$30</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$28</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="74">
   <si>
     <t>date</t>
   </si>
@@ -166,18 +166,6 @@
   </si>
   <si>
     <t>https://youtu.be/5sUzkrucL1E</t>
-  </si>
-  <si>
-    <t>NGS Pipelines</t>
-  </si>
-  <si>
-    <t>Adam Ameur</t>
-  </si>
-  <si>
-    <t>topics/other/slide_ngs_pipelines.pdf</t>
-  </si>
-  <si>
-    <t>https://youtu.be/6RBhfMvDkSI</t>
   </si>
   <si>
     <t>Variant-calling workflow</t>
@@ -709,10 +697,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F39" sqref="F39"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,7 +756,7 @@
         <v>11</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C2" s="1">
         <v>0.375</v>
@@ -820,7 +808,7 @@
         <v>13</v>
       </c>
       <c r="G4" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="I4" t="s">
         <v>18</v>
@@ -871,7 +859,7 @@
         <v>13</v>
       </c>
       <c r="G7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I7" t="s">
         <v>23</v>
@@ -914,7 +902,7 @@
         <v>13</v>
       </c>
       <c r="G9" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="I9" t="s">
         <v>28</v>
@@ -965,7 +953,7 @@
         <v>33</v>
       </c>
       <c r="G12" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>34</v>
@@ -1011,7 +999,7 @@
         <v>13</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I14" t="s">
         <v>40</v>
@@ -1025,7 +1013,7 @@
         <v>0.375</v>
       </c>
       <c r="D15" s="1">
-        <v>0.42708333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="E15" t="s">
         <v>42</v>
@@ -1040,252 +1028,218 @@
         <v>45</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C16" s="1">
-        <v>0.42708333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="1">
-        <v>0.45833333333333298</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="E16" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="17" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C17" s="1">
-        <v>0.45833333333333298</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D17" s="1">
-        <v>0.5</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="E17" t="s">
         <v>46</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" t="s">
         <v>47</v>
       </c>
-      <c r="H17" t="s">
+      <c r="J17" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C18" s="1">
-        <v>0.5</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="D18" s="1">
-        <v>0.54166666666666696</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="E18" t="s">
-        <v>19</v>
+        <v>46</v>
+      </c>
+      <c r="F18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="I18" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C19" s="1">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="D19" s="1">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="E19" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
         <v>50</v>
       </c>
-      <c r="F19" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="C20" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="E20" t="s">
         <v>51</v>
-      </c>
-      <c r="J19" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C20" s="1">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="D20" s="1">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="E20" t="s">
-        <v>50</v>
       </c>
       <c r="F20" t="s">
         <v>33</v>
       </c>
-      <c r="G20" t="s">
-        <v>73</v>
-      </c>
-      <c r="I20" t="s">
-        <v>53</v>
+      <c r="J20" s="2" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
+      <c r="C21" s="1">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E21" t="s">
+        <v>46</v>
+      </c>
+      <c r="F21" t="s">
+        <v>33</v>
+      </c>
+      <c r="G21" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>54</v>
-      </c>
       <c r="C22" s="1">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="D22" s="1">
-        <v>0.39583333333333298</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C23" s="1">
-        <v>0.39583333333333298</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D23" s="1">
-        <v>0.5</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="E23" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
-      </c>
-      <c r="G23" t="s">
-        <v>74</v>
+        <v>54</v>
+      </c>
+      <c r="H23" t="s">
+        <v>55</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C24" s="1">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" t="s">
+        <v>71</v>
+      </c>
+      <c r="I24" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.375</v>
+      </c>
+      <c r="D25" s="1">
         <v>0.5</v>
       </c>
-      <c r="D24" s="1">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="E24" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C25" s="1">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0.58333333333333304</v>
-      </c>
       <c r="E25" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="F25" t="s">
-        <v>58</v>
-      </c>
-      <c r="H25" t="s">
-        <v>59</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
+      </c>
+      <c r="G25" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C26" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="E26" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="C27" s="1">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D27" s="1">
         <v>0.58333333333333304</v>
       </c>
-      <c r="D26" s="1">
-        <v>0.70833333333333304</v>
-      </c>
-      <c r="E26" t="s">
-        <v>57</v>
-      </c>
-      <c r="F26" t="s">
-        <v>58</v>
-      </c>
-      <c r="G26" t="s">
-        <v>75</v>
-      </c>
-      <c r="I26" t="s">
+      <c r="E27" t="s">
+        <v>59</v>
+      </c>
+      <c r="F27" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" t="s">
+        <v>60</v>
+      </c>
+      <c r="J27" s="2" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>62</v>
-      </c>
-      <c r="C27" s="1">
-        <v>0.375</v>
-      </c>
-      <c r="D27" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="E27" t="s">
-        <v>57</v>
-      </c>
-      <c r="F27" t="s">
-        <v>58</v>
-      </c>
-      <c r="G27" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
       <c r="C28" s="1">
-        <v>0.5</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="D28" s="1">
-        <v>0.54166666666666696</v>
+        <v>0.59375</v>
       </c>
       <c r="E28" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C29" s="1">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="D29" s="1">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="E29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F28" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" t="s">
         <v>63</v>
       </c>
-      <c r="F29" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" t="s">
+      <c r="J28" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="J29" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="C30" s="1">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="D30" s="1">
-        <v>0.59375</v>
-      </c>
-      <c r="E30" t="s">
-        <v>66</v>
-      </c>
-      <c r="F30" t="s">
-        <v>33</v>
-      </c>
-      <c r="H30" t="s">
-        <v>67</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>
@@ -1297,12 +1251,11 @@
     <hyperlink ref="J12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="J13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="J15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="J17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="J19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J25" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="J29" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J30" r:id="rId13" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="J17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updated location, added dinner
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{684067E6-3C34-0444-B303-2698EDA25B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B24A2900-85BD-9E4E-B58D-029D5E429D8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4900" yWindow="3200" windowWidth="30160" windowHeight="16540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -106,9 +106,6 @@
     <t>link_room</t>
   </si>
   <si>
-    <t>18/03/2024</t>
-  </si>
-  <si>
     <t>Welcome</t>
   </si>
   <si>
@@ -145,9 +142,6 @@
     <t>topics/uppmax/intro/lab_uppmax_intro.html</t>
   </si>
   <si>
-    <t>19/03/2024</t>
-  </si>
-  <si>
     <t>File types in Bioinformatics</t>
   </si>
   <si>
@@ -196,9 +190,6 @@
     <t>topics/linux/lab_linux_advanced.html</t>
   </si>
   <si>
-    <t>20/03/2024</t>
-  </si>
-  <si>
     <t>NGS tech &amp; challenges</t>
   </si>
   <si>
@@ -223,9 +214,6 @@
     <t>topics/vc/lab_vc.html</t>
   </si>
   <si>
-    <t>21/03/2024</t>
-  </si>
-  <si>
     <t>GATK best practices</t>
   </si>
   <si>
@@ -247,9 +235,6 @@
     <t>topics/rnaseq/lab_rnaseq.html</t>
   </si>
   <si>
-    <t>22/03/2024</t>
-  </si>
-  <si>
     <t>Data management practices</t>
   </si>
   <si>
@@ -271,10 +256,25 @@
     <t>Elin Kronander / Stephan Nylinder</t>
   </si>
   <si>
-    <t>Dinner</t>
-  </si>
-  <si>
     <t>Linköping</t>
+  </si>
+  <si>
+    <t>25/11/2024</t>
+  </si>
+  <si>
+    <t>26/11/2024</t>
+  </si>
+  <si>
+    <t>27/11/2024</t>
+  </si>
+  <si>
+    <t>28/11/2024</t>
+  </si>
+  <si>
+    <t>29/11/2024</t>
+  </si>
+  <si>
+    <t>Course Dinner</t>
   </si>
 </sst>
 </file>
@@ -744,7 +744,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -799,10 +799,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
@@ -811,13 +811,13 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
@@ -828,16 +828,16 @@
         <v>0.4375</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
@@ -848,13 +848,13 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.2">
@@ -865,7 +865,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.2">
@@ -876,16 +876,16 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.2">
@@ -896,18 +896,18 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="C8" s="3">
         <v>0.375</v>
@@ -916,16 +916,16 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="J8" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -936,13 +936,13 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
@@ -953,16 +953,16 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.2">
@@ -973,7 +973,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.2">
@@ -984,19 +984,19 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="J12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.2">
@@ -1007,16 +1007,16 @@
         <v>0.625</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.2">
@@ -1027,18 +1027,18 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="C15" s="3">
         <v>0.375</v>
@@ -1047,16 +1047,16 @@
         <v>0.5</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -1067,7 +1067,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
@@ -1078,16 +1078,16 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
@@ -1098,18 +1098,18 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
       <c r="C19" s="3">
         <v>0.375</v>
@@ -1118,13 +1118,13 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
@@ -1135,10 +1135,10 @@
         <v>0.5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
@@ -1149,7 +1149,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1160,16 +1160,16 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
@@ -1180,13 +1180,13 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.2">
@@ -1197,12 +1197,12 @@
         <v>0.83333333333333337</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="C25" s="3">
         <v>0.375</v>
@@ -1211,10 +1211,10 @@
         <v>0.5</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
@@ -1225,7 +1225,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
@@ -1236,16 +1236,16 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="J27" s="4" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.2">
@@ -1256,16 +1256,16 @@
         <v>0.59375</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
UPPMAX intro lab -> HPC intro lab completed
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Lunch</t>
   </si>
   <si>
-    <t xml:space="preserve">Intro to high-performace computing</t>
+    <t xml:space="preserve">Intro to high-performance computing</t>
   </si>
   <si>
     <t xml:space="preserve">topics/hpc/intro/slide_hpc_intro.pdf</t>
@@ -688,7 +688,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Adapted HPC part to PDC
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -136,7 +136,7 @@
     <t xml:space="preserve">https://youtu.be/cxEtfKN91q4</t>
   </si>
   <si>
-    <t xml:space="preserve">topics/hpc/intro/lab_hpc_intro.html</t>
+    <t xml:space="preserve">topics/hpc/intro/lab_intro.html</t>
   </si>
   <si>
     <t xml:space="preserve">26/11/2024</t>
@@ -688,7 +688,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updated schedule, added TAs
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11018"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EA526A-3651-E040-BC4D-5CFE974C2A17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D3A014-0D83-9C4D-A8B3-739504DCE7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="1800" windowWidth="32860" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1580" yWindow="1680" windowWidth="32860" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
   <si>
     <t>date</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Roy Francis</t>
   </si>
   <si>
-    <t>Stephan Nylander</t>
-  </si>
-  <si>
     <t>Uppsala</t>
   </si>
   <si>
@@ -265,6 +262,33 @@
   </si>
   <si>
     <t>Diana Ekman</t>
+  </si>
+  <si>
+    <t>KG</t>
+  </si>
+  <si>
+    <t>KG,SS</t>
+  </si>
+  <si>
+    <t>JH,KG</t>
+  </si>
+  <si>
+    <t>GD,JH</t>
+  </si>
+  <si>
+    <t>GD,KG</t>
+  </si>
+  <si>
+    <t>AJ,SD</t>
+  </si>
+  <si>
+    <t>JH,SD</t>
+  </si>
+  <si>
+    <t>GD,SS</t>
+  </si>
+  <si>
+    <t>Elin Kronander</t>
   </si>
 </sst>
 </file>
@@ -617,7 +641,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4:G28"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -673,10 +697,10 @@
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
@@ -693,7 +717,9 @@
       <c r="H2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K2" s="4"/>
+      <c r="K2" s="1" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" s="3">
@@ -714,9 +740,6 @@
       <c r="J3" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="1" t="s">
-        <v>61</v>
-      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C4" s="3">
@@ -731,6 +754,9 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>17</v>
       </c>
@@ -779,16 +805,19 @@
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3">
         <v>0.375</v>
@@ -809,7 +838,7 @@
         <v>24</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.2">
@@ -825,6 +854,9 @@
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>69</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>25</v>
       </c>
@@ -871,7 +903,10 @@
         <v>29</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>70</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>30</v>
@@ -916,16 +951,19 @@
       <c r="F14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C15" s="3">
         <v>0.375</v>
@@ -946,7 +984,7 @@
         <v>40</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
@@ -971,7 +1009,7 @@
         <v>41</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>42</v>
@@ -991,7 +1029,10 @@
         <v>41</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>72</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>44</v>
@@ -999,10 +1040,10 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C19" s="3">
         <v>0.375</v>
@@ -1014,13 +1055,13 @@
         <v>45</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="J19" s="5" t="s">
         <v>46</v>
       </c>
       <c r="K19" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
@@ -1034,7 +1075,10 @@
         <v>41</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
@@ -1081,16 +1125,19 @@
       <c r="F23" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="G23" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="I23" s="1" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C24" s="3">
         <v>0.375</v>
@@ -1104,8 +1151,11 @@
       <c r="F24" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="G24" s="1" t="s">
+        <v>74</v>
+      </c>
       <c r="K24" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
@@ -1130,7 +1180,7 @@
         <v>51</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>52</v>
@@ -1148,6 +1198,9 @@
       </c>
       <c r="E27" s="1" t="s">
         <v>54</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>75</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
Added lab tour to schedule
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D3A014-0D83-9C4D-A8B3-739504DCE7D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCC8DDA9-540D-B345-BAF5-5DAFED4215CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1580" yWindow="1680" windowWidth="32860" windowHeight="20500" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$27</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$28</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="77">
   <si>
     <t>date</t>
   </si>
@@ -289,6 +289,9 @@
   </si>
   <si>
     <t>Elin Kronander</t>
+  </si>
+  <si>
+    <t>Lab tour</t>
   </si>
 </sst>
 </file>
@@ -307,29 +310,9 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
       <u/>
       <sz val="12"/>
       <color rgb="FF0563C1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="13"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -345,6 +328,31 @@
       <name val="Tahoma"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -366,16 +374,15 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -638,10 +645,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -737,7 +744,7 @@
       <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="J3" s="4" t="s">
         <v>16</v>
       </c>
     </row>
@@ -788,7 +795,7 @@
       <c r="H6" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -834,10 +841,10 @@
       <c r="H8" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="5" t="s">
         <v>60</v>
       </c>
     </row>
@@ -877,7 +884,7 @@
       <c r="H10" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
         <v>28</v>
       </c>
     </row>
@@ -914,7 +921,7 @@
       <c r="I12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -934,7 +941,7 @@
       <c r="H13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="J13" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -958,7 +965,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>63</v>
       </c>
@@ -969,61 +976,55 @@
         <v>0.375</v>
       </c>
       <c r="D15" s="3">
-        <v>0.5</v>
+        <v>0.48958333333333331</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="1" t="s">
         <v>38</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="K15" s="4" t="s">
+      <c r="K15" s="5" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
       <c r="C16" s="3">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D16" s="3">
         <v>0.5</v>
       </c>
-      <c r="D16" s="3">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="3">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D17" s="3">
-        <v>0.58333333333333304</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="J17" s="5" t="s">
-        <v>43</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D18" s="3">
         <v>0.58333333333333304</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.70833333333333304</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>41</v>
@@ -1031,93 +1032,93 @@
       <c r="F18" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>44</v>
+      <c r="H18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C19" s="3">
-        <v>0.375</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="D19" s="3">
-        <v>0.39583333333333298</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" s="4" t="s">
-        <v>60</v>
+      <c r="G19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>59</v>
+      </c>
       <c r="C20" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D20" s="3">
         <v>0.39583333333333298</v>
       </c>
-      <c r="D20" s="3">
-        <v>0.5</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="G20" s="1" t="s">
-        <v>73</v>
+      <c r="J20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C21" s="3">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="D21" s="3">
         <v>0.5</v>
       </c>
-      <c r="D21" s="3">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>41</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="3">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D22" s="3">
-        <v>0.60416666666666663</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D23" s="3">
         <v>0.60416666666666663</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.70833333333333304</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>47</v>
@@ -1125,25 +1126,19 @@
       <c r="F23" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>50</v>
+      <c r="H23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>59</v>
-      </c>
       <c r="C24" s="3">
-        <v>0.375</v>
+        <v>0.60416666666666663</v>
       </c>
       <c r="D24" s="3">
-        <v>0.5</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>47</v>
@@ -1154,58 +1149,84 @@
       <c r="G24" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="K24" s="4" t="s">
+      <c r="I24" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C25" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D25" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="K25" s="5" t="s">
         <v>60</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C25" s="3">
-        <v>0.5</v>
-      </c>
-      <c r="D25" s="3">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="3">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D26" s="3">
-        <v>0.58333333333333304</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J26" s="5" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C27" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D27" s="3">
         <v>0.58333333333333304</v>
       </c>
-      <c r="D27" s="3">
-        <v>0.59375</v>
-      </c>
       <c r="E27" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="F27" s="1" t="s">
         <v>75</v>
       </c>
       <c r="H27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="C28" s="3">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D28" s="3">
+        <v>0.59375</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J28" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1218,11 +1239,11 @@
     <hyperlink ref="J12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
     <hyperlink ref="J13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
     <hyperlink ref="J15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="J19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
-    <hyperlink ref="J22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
-    <hyperlink ref="J26" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
-    <hyperlink ref="J27" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="J18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="J27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="J28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Updated for Mar 2026, updated graphics
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11116"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A608EE4A-B45D-DC46-B580-E6512F47EE63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAB2F2-8384-9B48-9DD0-E0ED38DD6076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="620" windowWidth="31060" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3280" yWindow="1880" windowWidth="31060" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$29</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$27</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>date</t>
   </si>
@@ -96,9 +96,6 @@
     <t>link_room</t>
   </si>
   <si>
-    <t>17/11/2025</t>
-  </si>
-  <si>
     <t>Uppsala</t>
   </si>
   <si>
@@ -111,9 +108,6 @@
     <t>topics/other/slide_introduction.pdf</t>
   </si>
   <si>
-    <t>https://link.mazemap.com/ANPxhAhR</t>
-  </si>
-  <si>
     <t>Intro to Linux</t>
   </si>
   <si>
@@ -123,9 +117,6 @@
     <t>https://youtu.be/qYp8shSMJ-0</t>
   </si>
   <si>
-    <t>KG,SS,MP</t>
-  </si>
-  <si>
     <t>topics/linux/lab_linux_intro.html</t>
   </si>
   <si>
@@ -141,15 +132,9 @@
     <t>https://youtu.be/cxEtfKN91q4</t>
   </si>
   <si>
-    <t>KG,SS</t>
-  </si>
-  <si>
     <t>topics/hpc/intro/lab_intro.html</t>
   </si>
   <si>
-    <t>18/11/2025</t>
-  </si>
-  <si>
     <t>File types in Bioinformatics</t>
   </si>
   <si>
@@ -159,9 +144,6 @@
     <t>https://youtu.be/7MR1qUZQ94w</t>
   </si>
   <si>
-    <t>JH,KG</t>
-  </si>
-  <si>
     <t>topics/linux/lab_linux_filetypes.html</t>
   </si>
   <si>
@@ -180,9 +162,6 @@
     <t>Marcel Martin</t>
   </si>
   <si>
-    <t>GD,JH</t>
-  </si>
-  <si>
     <t>topics/other/slide_qc.pdf</t>
   </si>
   <si>
@@ -201,15 +180,9 @@
     <t>https://youtu.be/n3IpUHIodM8</t>
   </si>
   <si>
-    <t>GD,KG</t>
-  </si>
-  <si>
     <t>topics/linux/lab_linux_advanced.html</t>
   </si>
   <si>
-    <t>19/11/2025</t>
-  </si>
-  <si>
     <t>NGS tech &amp; challenges</t>
   </si>
   <si>
@@ -219,15 +192,9 @@
     <t>https://youtu.be/5sUzkrucL1E</t>
   </si>
   <si>
-    <t>Lab tour</t>
-  </si>
-  <si>
     <t>Variant-calling workflow</t>
   </si>
   <si>
-    <t>Marcus Mayrhofer</t>
-  </si>
-  <si>
     <t>topics/vc/slide_vc.pdf</t>
   </si>
   <si>
@@ -237,24 +204,15 @@
     <t>Diana Ekman</t>
   </si>
   <si>
-    <t>AJ,SD</t>
-  </si>
-  <si>
     <t>topics/vc/lab_vc.html</t>
   </si>
   <si>
-    <t>20/11/2025</t>
-  </si>
-  <si>
     <t>GATK best practices</t>
   </si>
   <si>
     <t>https://youtu.be/-cL0CI07-Es</t>
   </si>
   <si>
-    <t>JH,SD</t>
-  </si>
-  <si>
     <t>RNA-Seq workflow</t>
   </si>
   <si>
@@ -267,21 +225,12 @@
     <t>https://youtu.be/gC_nslHgSa8</t>
   </si>
   <si>
-    <t>GD,SS</t>
-  </si>
-  <si>
     <t>topics/rnaseq/lab_rnaseq.html</t>
   </si>
   <si>
-    <t>21/11/2025</t>
-  </si>
-  <si>
     <t>Data management practices</t>
   </si>
   <si>
-    <t>Elin Kronander</t>
-  </si>
-  <si>
     <t>topics/other/slide_data_management.pdf</t>
   </si>
   <si>
@@ -297,10 +246,22 @@
     <t>https://youtu.be/4HbSAEU5iBM</t>
   </si>
   <si>
-    <t>Course Dinner at Koh Phangan, Uppsala</t>
-  </si>
-  <si>
     <t>https://drive.google.com/file/d/15vG6VXaSL7lWNPQ6Sdn6-cxPWYHf2AAv/view?usp=sharing</t>
+  </si>
+  <si>
+    <t>02/03/2026</t>
+  </si>
+  <si>
+    <t>03/03/2026</t>
+  </si>
+  <si>
+    <t>04/03/2026</t>
+  </si>
+  <si>
+    <t>05/03/2026</t>
+  </si>
+  <si>
+    <t>06/03/2026</t>
   </si>
 </sst>
 </file>
@@ -643,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -702,10 +663,10 @@
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>12</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
@@ -714,16 +675,13 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -734,16 +692,16 @@
         <v>0.4375</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>17</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -754,16 +712,13 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -774,7 +729,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -785,16 +740,16 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -805,24 +760,21 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>23</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>28</v>
+        <v>63</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C8" s="3">
         <v>0.375</v>
@@ -831,20 +783,18 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K8" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="K8" s="5"/>
     </row>
     <row r="9" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C9" s="3">
@@ -854,16 +804,13 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>32</v>
+        <v>13</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -874,16 +821,16 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -894,7 +841,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -905,22 +852,19 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -931,16 +875,16 @@
         <v>0.625</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -951,292 +895,240 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C15" s="3">
         <v>0.375</v>
       </c>
       <c r="D15" s="3">
-        <v>0.48958333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="K15" s="5" t="s">
-        <v>16</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="B16" s="2"/>
       <c r="C16" s="3">
-        <v>0.48958333333333298</v>
+        <v>0.5</v>
       </c>
       <c r="D16" s="3">
-        <v>0.5</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="J16" s="4"/>
-      <c r="K16" s="5"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
-        <v>0.5</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D17" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>22</v>
+        <v>43</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="D18" s="3">
-        <v>0.58333333333333304</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="J18" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A19" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C19" s="3">
-        <v>0.58333333333333304</v>
+        <v>0.375</v>
       </c>
       <c r="D19" s="3">
-        <v>0.70833333333333304</v>
+        <v>0.39583333333333298</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>59</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="K19" s="5"/>
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C20" s="3">
-        <v>0.75</v>
+        <v>0.39583333333333298</v>
       </c>
       <c r="D20" s="3">
-        <v>0.875</v>
+        <v>0.5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>78</v>
+        <v>43</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C21" s="3">
-        <v>0.375</v>
+        <v>0.5</v>
       </c>
       <c r="D21" s="3">
-        <v>0.39583333333333298</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="K21" s="5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
-        <v>0.39583333333333298</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D22" s="3">
-        <v>0.5</v>
+        <v>0.60416666666666696</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="J22" s="4" t="s">
         <v>53</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
+        <v>0.60416666666666696</v>
+      </c>
+      <c r="D23" s="3">
+        <v>0.70833333333333304</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F23" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I23" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A24" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D24" s="3">
         <v>0.5</v>
       </c>
-      <c r="D23" s="3">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="C24" s="3">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="D24" s="3">
-        <v>0.60416666666666696</v>
-      </c>
       <c r="E24" s="1" t="s">
-        <v>64</v>
+        <v>50</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>67</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="K24" s="5"/>
     </row>
     <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C25" s="3">
-        <v>0.60416666666666696</v>
+        <v>0.5</v>
       </c>
       <c r="D25" s="3">
-        <v>0.70833333333333304</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="I25" s="1" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>12</v>
-      </c>
       <c r="C26" s="3">
-        <v>0.375</v>
+        <v>0.54166666666666696</v>
       </c>
       <c r="D26" s="3">
-        <v>0.5</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G26" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="K26" s="5" t="s">
-        <v>16</v>
+        <v>55</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C27" s="3">
-        <v>0.5</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="D27" s="3">
-        <v>0.54166666666666696</v>
+        <v>0.59375</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="C28" s="3">
-        <v>0.54166666666666696</v>
-      </c>
-      <c r="D28" s="3">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H28" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="C29" s="3">
-        <v>0.58333333333333304</v>
-      </c>
-      <c r="D29" s="3">
-        <v>0.59375</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F29" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="H29" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>77</v>
+        <v>58</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1248,11 +1140,11 @@
     <hyperlink ref="J12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="J13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="J15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="J18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="J21" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J24" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J28" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="J29" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J26" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J27" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
Merged about to info, Corrected room
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10FAB2F2-8384-9B48-9DD0-E0ED38DD6076}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521C14AA-0F5E-5343-AD4D-E4702D0C5B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3280" yWindow="1880" windowWidth="31060" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>link_room</t>
   </si>
   <si>
-    <t>Uppsala</t>
-  </si>
-  <si>
     <t>Welcome</t>
   </si>
   <si>
@@ -262,6 +259,9 @@
   </si>
   <si>
     <t>06/03/2026</t>
+  </si>
+  <si>
+    <t>Online</t>
   </si>
 </sst>
 </file>
@@ -607,7 +607,7 @@
   <dimension ref="A1:K27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -663,10 +663,10 @@
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="C2" s="3">
         <v>0.375</v>
@@ -675,13 +675,13 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -692,16 +692,16 @@
         <v>0.4375</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="J3" s="4" t="s">
         <v>16</v>
-      </c>
-      <c r="J3" s="4" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -712,13 +712,13 @@
         <v>0.5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -729,7 +729,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -740,16 +740,16 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="4" t="s">
         <v>21</v>
-      </c>
-      <c r="J6" s="4" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -760,21 +760,21 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="C8" s="3">
         <v>0.375</v>
@@ -783,16 +783,16 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H8" s="1" t="s">
+      <c r="J8" s="4" t="s">
         <v>25</v>
-      </c>
-      <c r="J8" s="4" t="s">
-        <v>26</v>
       </c>
       <c r="K8" s="5"/>
     </row>
@@ -804,13 +804,13 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -821,16 +821,16 @@
         <v>0.5</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H10" s="1" t="s">
+      <c r="J10" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="J10" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -841,7 +841,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -852,19 +852,19 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="I12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="4" t="s">
         <v>34</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -875,16 +875,16 @@
         <v>0.625</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="1" t="s">
+      <c r="J13" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="J13" s="4" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -895,21 +895,21 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I14" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="C15" s="3">
         <v>0.375</v>
@@ -918,16 +918,16 @@
         <v>0.5</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="J15" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>42</v>
       </c>
       <c r="K15" s="5"/>
     </row>
@@ -939,7 +939,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -950,16 +950,16 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="1" t="s">
+      <c r="J17" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -970,21 +970,21 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F18" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>11</v>
+        <v>66</v>
       </c>
       <c r="C19" s="3">
         <v>0.375</v>
@@ -993,13 +993,13 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="E19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J19" s="4" t="s">
         <v>48</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>49</v>
       </c>
       <c r="K19" s="5"/>
     </row>
@@ -1011,10 +1011,10 @@
         <v>0.5</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1025,7 +1025,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1036,16 +1036,16 @@
         <v>0.60416666666666696</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F22" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="H22" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H22" s="1" t="s">
+      <c r="J22" s="4" t="s">
         <v>52</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1056,21 +1056,21 @@
         <v>0.70833333333333304</v>
       </c>
       <c r="E23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F23" s="1" t="s">
-        <v>51</v>
-      </c>
       <c r="I23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>66</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>11</v>
       </c>
       <c r="C24" s="3">
         <v>0.375</v>
@@ -1079,10 +1079,10 @@
         <v>0.5</v>
       </c>
       <c r="E24" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="K24" s="5"/>
     </row>
@@ -1094,7 +1094,7 @@
         <v>0.54166666666666696</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1105,13 +1105,13 @@
         <v>0.58333333333333304</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H26" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H26" s="1" t="s">
+      <c r="J26" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
@@ -1122,13 +1122,13 @@
         <v>0.59375</v>
       </c>
       <c r="E27" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="J27" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="J27" s="4" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated schedule with TAs
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/royfr474/github/workshop-ngsintro/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C83D3DF-F0AA-8C43-A118-64CCD1C27468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F117B47-D0B6-774A-BA80-B634EBA306E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3280" yWindow="1880" windowWidth="31060" windowHeight="18920" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$27</definedName>
+    <definedName name="schedule" localSheetId="0">Sheet1!$A$1:$K$28</definedName>
   </definedNames>
   <calcPr calcId="0" iterateDelta="1E-4"/>
   <extLst>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="79">
   <si>
     <t>date</t>
   </si>
@@ -258,13 +258,46 @@
     <t>Online</t>
   </si>
   <si>
-    <t>NGS technologies &amp; pipelines</t>
-  </si>
-  <si>
-    <t>Johanna Lagensjö &amp; Christian Tellgren-Roth</t>
-  </si>
-  <si>
-    <t>SS</t>
+    <t>KG, RF, MP</t>
+  </si>
+  <si>
+    <t>KG, JH</t>
+  </si>
+  <si>
+    <t>JH</t>
+  </si>
+  <si>
+    <t>ML, MP</t>
+  </si>
+  <si>
+    <t>ML, AJ</t>
+  </si>
+  <si>
+    <t>SS, MP</t>
+  </si>
+  <si>
+    <t>DA, SS, MP</t>
+  </si>
+  <si>
+    <t>Maria Vrettou</t>
+  </si>
+  <si>
+    <t>Dag Ahrén</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>NGS technologies</t>
+  </si>
+  <si>
+    <t>NGS pipelines</t>
+  </si>
+  <si>
+    <t>Christian Tellgren-Roth</t>
+  </si>
+  <si>
+    <t>Johanna Lagensjö</t>
   </si>
 </sst>
 </file>
@@ -338,13 +371,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -607,10 +641,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K27"/>
+  <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+      <selection activeCell="G35" sqref="G35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -620,8 +654,8 @@
     <col min="3" max="3" width="9.83203125" style="1" customWidth="1"/>
     <col min="4" max="4" width="9" style="1" customWidth="1"/>
     <col min="5" max="5" width="24.6640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="37.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="35.5" style="1" customWidth="1"/>
     <col min="9" max="9" width="31.5" style="1" customWidth="1"/>
     <col min="10" max="10" width="29.5" style="1" customWidth="1"/>
@@ -720,6 +754,9 @@
       <c r="F4" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G4" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="I4" s="1" t="s">
         <v>17</v>
       </c>
@@ -768,6 +805,9 @@
       <c r="F7" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G7" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="I7" s="1" t="s">
         <v>22</v>
       </c>
@@ -812,6 +852,9 @@
       <c r="F9" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G9" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="I9" s="1" t="s">
         <v>26</v>
       </c>
@@ -860,6 +903,9 @@
       <c r="F12" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="G12" s="1" t="s">
+        <v>67</v>
+      </c>
       <c r="H12" s="1" t="s">
         <v>32</v>
       </c>
@@ -903,6 +949,9 @@
       <c r="F14" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="G14" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="I14" s="1" t="s">
         <v>38</v>
       </c>
@@ -918,13 +967,13 @@
         <v>0.375</v>
       </c>
       <c r="D15" s="3">
-        <v>0.5</v>
+        <v>0.41666666666666669</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>66</v>
+        <v>78</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>58</v>
@@ -935,42 +984,39 @@
       <c r="K15" s="5"/>
     </row>
     <row r="16" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="B16" s="2"/>
       <c r="C16" s="3">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D16" s="3">
         <v>0.5</v>
       </c>
-      <c r="D16" s="3">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E16" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J16" s="4"/>
+      <c r="K16" s="5"/>
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C17" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D17" s="3">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D17" s="3">
-        <v>0.58333333333333304</v>
-      </c>
       <c r="E17" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C18" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D18" s="3">
         <v>0.58333333333333304</v>
-      </c>
-      <c r="D18" s="3">
-        <v>0.70833333333333304</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>40</v>
@@ -978,85 +1024,91 @@
       <c r="F18" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>44</v>
+      <c r="H18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C19" s="3">
-        <v>0.375</v>
+        <v>0.58333333333333304</v>
       </c>
       <c r="D19" s="3">
-        <v>0.39583333333333298</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="J19" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="K19" s="5"/>
+      <c r="G19" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A20" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="C20" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D20" s="3">
         <v>0.39583333333333298</v>
       </c>
-      <c r="D20" s="3">
-        <v>0.5</v>
-      </c>
       <c r="E20" s="1" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="J20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="5"/>
     </row>
     <row r="21" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C21" s="3">
+        <v>0.39583333333333298</v>
+      </c>
+      <c r="D21" s="3">
         <v>0.5</v>
       </c>
-      <c r="D21" s="3">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E21" s="1" t="s">
-        <v>18</v>
+        <v>40</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="3">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D22" s="3">
-        <v>0.60416666666666696</v>
-      </c>
       <c r="E22" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C23" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D23" s="3">
         <v>0.60416666666666696</v>
-      </c>
-      <c r="D23" s="3">
-        <v>0.70833333333333304</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>47</v>
@@ -1064,25 +1116,19 @@
       <c r="F23" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G23" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>51</v>
+      <c r="H23" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>64</v>
-      </c>
       <c r="C24" s="3">
-        <v>0.375</v>
+        <v>0.60416666666666696</v>
       </c>
       <c r="D24" s="3">
-        <v>0.5</v>
+        <v>0.70833333333333304</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>47</v>
@@ -1091,53 +1137,99 @@
         <v>48</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="K24" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
     <row r="25" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>64</v>
+      </c>
       <c r="C25" s="3">
+        <v>0.375</v>
+      </c>
+      <c r="D25" s="3">
         <v>0.5</v>
       </c>
-      <c r="D25" s="3">
-        <v>0.54166666666666696</v>
-      </c>
       <c r="E25" s="1" t="s">
-        <v>18</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="K25" s="5"/>
     </row>
     <row r="26" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C26" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="D26" s="3">
         <v>0.54166666666666696</v>
       </c>
-      <c r="D26" s="3">
-        <v>0.58333333333333304</v>
-      </c>
       <c r="E26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="J26" s="4" t="s">
-        <v>54</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="C27" s="3">
+        <v>0.54166666666666696</v>
+      </c>
+      <c r="D27" s="3">
         <v>0.58333333333333304</v>
       </c>
-      <c r="D27" s="3">
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="C28" s="3">
+        <v>0.58333333333333304</v>
+      </c>
+      <c r="D28" s="3">
         <v>0.59375</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="H27" s="1" t="s">
+      <c r="F28" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="H28" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="J27" s="4" t="s">
+      <c r="J28" s="4" t="s">
         <v>57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C29" s="6">
+        <v>0.59375</v>
+      </c>
+      <c r="D29" s="6">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1149,11 +1241,11 @@
     <hyperlink ref="J12" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
     <hyperlink ref="J13" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
     <hyperlink ref="J15" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
-    <hyperlink ref="J17" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
-    <hyperlink ref="J19" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
-    <hyperlink ref="J22" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
-    <hyperlink ref="J26" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
-    <hyperlink ref="J27" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="J18" r:id="rId8" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="J20" r:id="rId9" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="J23" r:id="rId10" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="J27" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="J28" r:id="rId12" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>